<commit_message>
Removed Matlab index from the analysis (not from data) Worked on input to 2 over 3
</commit_message>
<xml_diff>
--- a/aru.27.123a4/data/GSS_indices270120_AK.xlsx
+++ b/aru.27.123a4/data/GSS_indices270120_AK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\DLS\SPiCT\Benchmark2020\wk_WKGSS\aru.27.123a4\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944D88E3-3A21-40CF-99A4-ECBAE46B9DB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778F63CD-7904-4D28-BEBF-3EB20DB8E3F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -443,29 +443,28 @@
   <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.89453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="5.9453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.15625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.9453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.9453125" customWidth="1"/>
-    <col min="8" max="8" width="10.62890625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.62890625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.15625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.89453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.83984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="1017" width="8.68359375" customWidth="1"/>
-    <col min="1018" max="1023" width="11.5234375"/>
+    <col min="12" max="12" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="1017" width="8.7109375" customWidth="1"/>
+    <col min="1018" max="1023" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +514,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1984</v>
       </c>
@@ -540,7 +539,7 @@
         <v>9886.6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1985</v>
       </c>
@@ -565,7 +564,7 @@
         <v>16055.9</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1986</v>
       </c>
@@ -590,7 +589,7 @@
         <v>14947.4</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1987</v>
       </c>
@@ -615,7 +614,7 @@
         <v>12524.1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1988</v>
       </c>
@@ -642,7 +641,7 @@
         <v>6970.7</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1989</v>
       </c>
@@ -669,7 +668,7 @@
         <v>5912.5</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1990</v>
       </c>
@@ -705,7 +704,7 @@
         <v>1680000</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1991</v>
       </c>
@@ -741,7 +740,7 @@
         <v>1800000</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1992</v>
       </c>
@@ -777,7 +776,7 @@
         <v>1610000</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1993</v>
       </c>
@@ -804,7 +803,7 @@
         <v>7525.9</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1994</v>
       </c>
@@ -831,7 +830,7 @@
         <v>4380</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1995</v>
       </c>
@@ -858,7 +857,7 @@
         <v>3633.8</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1996</v>
       </c>
@@ -885,7 +884,7 @@
         <v>1851.3</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1997</v>
       </c>
@@ -912,7 +911,7 @@
         <v>3212</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1998</v>
       </c>
@@ -939,7 +938,7 @@
         <v>6406.8</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1999</v>
       </c>
@@ -966,7 +965,7 @@
         <v>4231</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2000</v>
       </c>
@@ -996,7 +995,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2001</v>
       </c>
@@ -1026,7 +1025,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2002</v>
       </c>
@@ -1056,7 +1055,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2003</v>
       </c>
@@ -1080,7 +1079,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2004</v>
       </c>
@@ -1112,7 +1111,7 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>2005</v>
       </c>
@@ -1144,7 +1143,7 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2006</v>
       </c>
@@ -1174,7 +1173,7 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2007</v>
       </c>
@@ -1204,7 +1203,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2008</v>
       </c>
@@ -1234,7 +1233,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2009</v>
       </c>
@@ -1266,12 +1265,14 @@
       <c r="J27" s="1">
         <v>427959</v>
       </c>
-      <c r="K27" s="1"/>
+      <c r="K27" s="1">
+        <v>443885.8</v>
+      </c>
       <c r="O27">
         <v>427959</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2010</v>
       </c>
@@ -1301,7 +1302,7 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2011</v>
       </c>
@@ -1337,7 +1338,7 @@
         <v>17.345459999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2012</v>
       </c>
@@ -1382,7 +1383,7 @@
         <v>322646</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2013</v>
       </c>
@@ -1418,7 +1419,7 @@
         <v>18.23639</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2014</v>
       </c>
@@ -1463,7 +1464,7 @@
         <v>508349</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2015</v>
       </c>
@@ -1499,7 +1500,7 @@
         <v>14.277710000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2016</v>
       </c>
@@ -1538,7 +1539,7 @@
         <v>549935</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2017</v>
       </c>
@@ -1574,7 +1575,7 @@
         <v>12.49779</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2018</v>
       </c>
@@ -1619,7 +1620,7 @@
         <v>344834</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2019</v>
       </c>
@@ -1639,10 +1640,10 @@
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G39" s="1"/>
     </row>
   </sheetData>

</xml_diff>